<commit_message>
Added GDP and cons and looked into nonstationarity a little bit
So it seems to me that the IT series is super sensitive to whether we
take logs or not - if we do, we obtain stationarity!! That changes IRFs
in meaningful ways, however. Need to discuss about that!
</commit_message>
<xml_diff>
--- a/dataset_23_sept_2017.xlsx
+++ b/dataset_23_sept_2017.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="291">
   <si>
     <t>date</t>
   </si>
@@ -889,6 +889,12 @@
   </si>
   <si>
     <t>IT investment</t>
+  </si>
+  <si>
+    <t>real GDP</t>
+  </si>
+  <si>
+    <t>real consumption (personal cons expenditures)</t>
   </si>
 </sst>
 </file>
@@ -938,7 +944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -947,6 +953,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1262,10 +1269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1999"/>
+  <dimension ref="A1:H1999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="I276" sqref="I276"/>
+    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
+      <selection activeCell="H283" sqref="H283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1273,9 +1280,10 @@
     <col min="2" max="2" width="8.83203125" style="3"/>
     <col min="4" max="4" width="8.83203125" style="3"/>
     <col min="6" max="6" width="8.83203125" style="3"/>
+    <col min="8" max="8" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1294,8 +1302,14 @@
       <c r="F1" s="3" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>289</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1306,8 +1320,14 @@
       <c r="F2" s="5">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="6">
+        <v>1934.5</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1199.4000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1320,8 +1340,14 @@
       <c r="F3" s="5">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="6">
+        <v>1932.3</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1219.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1334,8 +1360,14 @@
       <c r="F4" s="5">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="6">
+        <v>1930.3</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1223.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1348,8 +1380,14 @@
       <c r="F5" s="5">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="6">
+        <v>1960.7</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1223.5999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1362,8 +1400,14 @@
       <c r="F6" s="5">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="6">
+        <v>1989.5</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1229.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1376,8 +1420,14 @@
       <c r="F7" s="5">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="6">
+        <v>2021.9</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1244.0999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1390,8 +1440,14 @@
       <c r="F8" s="5">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="6">
+        <v>2033.2</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1245.9000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1404,8 +1460,14 @@
       <c r="F9" s="5">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="6">
+        <v>2035.3</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1255.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1418,8 +1480,14 @@
       <c r="F10" s="5">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="6">
+        <v>2007.5</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1257.9000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1432,8 +1500,14 @@
       <c r="F11" s="5">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="6">
+        <v>2000.8</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1277.0999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1446,8 +1520,14 @@
       <c r="F12" s="5">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="6">
+        <v>2022.8</v>
+      </c>
+      <c r="H12" s="5">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1460,8 +1540,14 @@
       <c r="F13" s="5">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="6">
+        <v>2004.7</v>
+      </c>
+      <c r="H13" s="5">
+        <v>1298.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1474,8 +1560,14 @@
       <c r="F14" s="5">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="6">
+        <v>2084.6</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1320.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1488,8 +1580,14 @@
       <c r="F15" s="5">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="6">
+        <v>2147.6</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1342.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1502,8 +1600,14 @@
       <c r="F16" s="5">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="6">
+        <v>2230.4</v>
+      </c>
+      <c r="H16" s="5">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1516,8 +1620,14 @@
       <c r="F17" s="5">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="6">
+        <v>2273.4</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1368.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1530,8 +1640,14 @@
       <c r="F18" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="6">
+        <v>2304.5</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1401.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1544,8 +1660,14 @@
       <c r="F19" s="5">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="6">
+        <v>2344.5</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1361.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1558,8 +1680,14 @@
       <c r="F20" s="5">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="6">
+        <v>2392.8000000000002</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1377.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1572,8 +1700,14 @@
       <c r="F21" s="5">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" s="6">
+        <v>2398.1</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1385.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1586,8 +1720,14 @@
       <c r="F22" s="5">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" s="6">
+        <v>2423.5</v>
+      </c>
+      <c r="H22" s="5">
+        <v>1388.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1600,8 +1740,14 @@
       <c r="F23" s="5">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" s="6">
+        <v>2428.5</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1416.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1614,8 +1760,14 @@
       <c r="F24" s="5">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="6">
+        <v>2446.1</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1628,8 +1780,14 @@
       <c r="F25" s="5">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" s="6">
+        <v>2526.4</v>
+      </c>
+      <c r="H25" s="5">
+        <v>1473.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1642,8 +1800,14 @@
       <c r="F26" s="5">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" s="6">
+        <v>2573.4</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1490.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1656,8 +1820,14 @@
       <c r="F27" s="5">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" s="6">
+        <v>2593.5</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1499.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1670,8 +1840,14 @@
       <c r="F28" s="5">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" s="6">
+        <v>2578.9</v>
+      </c>
+      <c r="H28" s="5">
+        <v>1496.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1684,8 +1860,14 @@
       <c r="F29" s="5">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" s="6">
+        <v>2539.8000000000002</v>
+      </c>
+      <c r="H29" s="5">
+        <v>1486.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1698,8 +1880,14 @@
       <c r="F30" s="5">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="6">
+        <v>2528</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1491.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1712,8 +1900,14 @@
       <c r="F31" s="5">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" s="6">
+        <v>2530.6999999999998</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1511.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1726,8 +1920,14 @@
       <c r="F32" s="5">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" s="6">
+        <v>2559.4</v>
+      </c>
+      <c r="H32" s="5">
+        <v>1531.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1740,8 +1940,14 @@
       <c r="F33" s="5">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" s="6">
+        <v>2609.3000000000002</v>
+      </c>
+      <c r="H33" s="5">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1754,8 +1960,14 @@
       <c r="F34" s="5">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34" s="6">
+        <v>2683.8</v>
+      </c>
+      <c r="H34" s="5">
+        <v>1599.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1768,8 +1980,14 @@
       <c r="F35" s="5">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35" s="6">
+        <v>2727.5</v>
+      </c>
+      <c r="H35" s="5">
+        <v>1629.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1782,8 +2000,14 @@
       <c r="F36" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36" s="6">
+        <v>2764.1</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1649.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1796,8 +2020,14 @@
       <c r="F37" s="5">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37" s="6">
+        <v>2780.8</v>
+      </c>
+      <c r="H37" s="5">
+        <v>1670.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1810,8 +2040,14 @@
       <c r="F38" s="5">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38" s="6">
+        <v>2770</v>
+      </c>
+      <c r="H38" s="5">
+        <v>1673.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1824,8 +2060,14 @@
       <c r="F39" s="5">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39" s="6">
+        <v>2792.9</v>
+      </c>
+      <c r="H39" s="5">
+        <v>1678.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1838,8 +2080,14 @@
       <c r="F40" s="5">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40" s="6">
+        <v>2790.6</v>
+      </c>
+      <c r="H40" s="5">
+        <v>1682.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1852,8 +2100,14 @@
       <c r="F41" s="5">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41" s="6">
+        <v>2836.2</v>
+      </c>
+      <c r="H41" s="5">
+        <v>1705.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1866,8 +2120,14 @@
       <c r="F42" s="5">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42" s="6">
+        <v>2854.5</v>
+      </c>
+      <c r="H42" s="5">
+        <v>1717.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1880,8 +2140,14 @@
       <c r="F43" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43" s="6">
+        <v>2848.2</v>
+      </c>
+      <c r="H43" s="5">
+        <v>1720.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1894,8 +2160,14 @@
       <c r="F44" s="5">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44" s="6">
+        <v>2875.9</v>
+      </c>
+      <c r="H44" s="5">
+        <v>1734.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1908,8 +2180,14 @@
       <c r="F45" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45" s="6">
+        <v>2846.4</v>
+      </c>
+      <c r="H45" s="5">
+        <v>1734.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1922,8 +2200,14 @@
       <c r="F46" s="5">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46" s="6">
+        <v>2772.7</v>
+      </c>
+      <c r="H46" s="5">
+        <v>1711.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1936,8 +2220,14 @@
       <c r="F47" s="5">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47" s="6">
+        <v>2790.9</v>
+      </c>
+      <c r="H47" s="5">
+        <v>1725.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1950,8 +2240,14 @@
       <c r="F48" s="5">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48" s="6">
+        <v>2855.5</v>
+      </c>
+      <c r="H48" s="5">
+        <v>1753.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1964,8 +2260,14 @@
       <c r="F49" s="5">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49" s="6">
+        <v>2922.3</v>
+      </c>
+      <c r="H49" s="5">
+        <v>1777.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1978,8 +2280,14 @@
       <c r="F50" s="5">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50" s="6">
+        <v>2976.6</v>
+      </c>
+      <c r="H50" s="5">
+        <v>1809.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1992,8 +2300,14 @@
       <c r="F51" s="5">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" s="6">
+        <v>3049</v>
+      </c>
+      <c r="H51" s="5">
+        <v>1837.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2006,8 +2320,14 @@
       <c r="F52" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52" s="6">
+        <v>3043.1</v>
+      </c>
+      <c r="H52" s="5">
+        <v>1856.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2020,8 +2340,14 @@
       <c r="F53" s="5">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53" s="6">
+        <v>3055.1</v>
+      </c>
+      <c r="H53" s="5">
+        <v>1858.6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2034,8 +2360,14 @@
       <c r="F54" s="5">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54" s="6">
+        <v>3123.2</v>
+      </c>
+      <c r="H54" s="5">
+        <v>1876.3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2048,8 +2380,14 @@
       <c r="F55" s="5">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55" s="6">
+        <v>3111.3</v>
+      </c>
+      <c r="H55" s="5">
+        <v>1900.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2062,8 +2400,14 @@
       <c r="F56" s="5">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56" s="6">
+        <v>3119.1</v>
+      </c>
+      <c r="H56" s="5">
+        <v>1892.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2076,8 +2420,14 @@
       <c r="F57" s="5">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57" s="6">
+        <v>3081.3</v>
+      </c>
+      <c r="H57" s="5">
+        <v>1894.9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2090,8 +2440,14 @@
       <c r="F58" s="5">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58" s="6">
+        <v>3102.3</v>
+      </c>
+      <c r="H58" s="5">
+        <v>1894.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2104,8 +2460,14 @@
       <c r="F59" s="5">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59" s="6">
+        <v>3159.9</v>
+      </c>
+      <c r="H59" s="5">
+        <v>1922.6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2118,8 +2480,14 @@
       <c r="F60" s="5">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60" s="6">
+        <v>3212.6</v>
+      </c>
+      <c r="H60" s="5">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2132,8 +2500,14 @@
       <c r="F61" s="5">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61" s="6">
+        <v>3277.7</v>
+      </c>
+      <c r="H61" s="5">
+        <v>1970.7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2146,8 +2520,14 @@
       <c r="F62" s="5">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62" s="6">
+        <v>3336.8</v>
+      </c>
+      <c r="H62" s="5">
+        <v>1991.7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2160,8 +2540,14 @@
       <c r="F63" s="5">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63" s="6">
+        <v>3372.7</v>
+      </c>
+      <c r="H63" s="5">
+        <v>2016.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2174,8 +2560,14 @@
       <c r="F64" s="5">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64" s="6">
+        <v>3404.8</v>
+      </c>
+      <c r="H64" s="5">
+        <v>2032.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2188,8 +2580,14 @@
       <c r="F65" s="5">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65" s="6">
+        <v>3418</v>
+      </c>
+      <c r="H65" s="5">
+        <v>2061.3000000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2202,8 +2600,14 @@
       <c r="F66" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66" s="6">
+        <v>3456.1</v>
+      </c>
+      <c r="H66" s="5">
+        <v>2075.1999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2216,8 +2620,14 @@
       <c r="F67" s="5">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67" s="6">
+        <v>3501.1</v>
+      </c>
+      <c r="H67" s="5">
+        <v>2095.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2230,8 +2640,14 @@
       <c r="F68" s="5">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68" s="6">
+        <v>3569.5</v>
+      </c>
+      <c r="H68" s="5">
+        <v>2123.6999999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2244,8 +2660,14 @@
       <c r="F69" s="5">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69" s="6">
+        <v>3595</v>
+      </c>
+      <c r="H69" s="5">
+        <v>2141.4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2258,8 +2680,14 @@
       <c r="F70" s="5">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70" s="6">
+        <v>3672.7</v>
+      </c>
+      <c r="H70" s="5">
+        <v>2183.6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2272,8 +2700,14 @@
       <c r="F71" s="5">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71" s="6">
+        <v>3716.4</v>
+      </c>
+      <c r="H71" s="5">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2286,8 +2720,14 @@
       <c r="F72" s="5">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72" s="6">
+        <v>3766.9</v>
+      </c>
+      <c r="H72" s="5">
+        <v>2262.8000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2300,8 +2740,14 @@
       <c r="F73" s="5">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73" s="6">
+        <v>3780.2</v>
+      </c>
+      <c r="H73" s="5">
+        <v>2269.1999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2314,8 +2760,14 @@
       <c r="F74" s="5">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74" s="6">
+        <v>3873.5</v>
+      </c>
+      <c r="H74" s="5">
+        <v>2319.8000000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2328,8 +2780,14 @@
       <c r="F75" s="5">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75" s="6">
+        <v>3926.4</v>
+      </c>
+      <c r="H75" s="5">
+        <v>2345.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2342,8 +2800,14 @@
       <c r="F76" s="5">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76" s="6">
+        <v>4006.2</v>
+      </c>
+      <c r="H76" s="5">
+        <v>2385.9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2356,8 +2820,14 @@
       <c r="F77" s="5">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77" s="6">
+        <v>4100.6000000000004</v>
+      </c>
+      <c r="H77" s="5">
+        <v>2452.9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2370,8 +2840,14 @@
       <c r="F78" s="5">
         <v>9.8000000000000007</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78" s="6">
+        <v>4201.8999999999996</v>
+      </c>
+      <c r="H78" s="5">
+        <v>2489.1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2384,8 +2860,14 @@
       <c r="F79" s="5">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79" s="6">
+        <v>4219.1000000000004</v>
+      </c>
+      <c r="H79" s="5">
+        <v>2495.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2398,8 +2880,14 @@
       <c r="F80" s="5">
         <v>10.9</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80" s="6">
+        <v>4249.2</v>
+      </c>
+      <c r="H80" s="5">
+        <v>2523.8000000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2412,8 +2900,14 @@
       <c r="F81" s="5">
         <v>11.4</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81" s="6">
+        <v>4285.6000000000004</v>
+      </c>
+      <c r="H81" s="5">
+        <v>2534.1999999999998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2426,8 +2920,14 @@
       <c r="F82" s="5">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="G82" s="6">
+        <v>4324.8999999999996</v>
+      </c>
+      <c r="H82" s="5">
+        <v>2548.9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2440,8 +2940,14 @@
       <c r="F83" s="5">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="G83" s="6">
+        <v>4328.7</v>
+      </c>
+      <c r="H83" s="5">
+        <v>2583.6999999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2454,8 +2960,14 @@
       <c r="F84" s="5">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="G84" s="6">
+        <v>4366.1000000000004</v>
+      </c>
+      <c r="H84" s="5">
+        <v>2596.9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2468,8 +2980,14 @@
       <c r="F85" s="5">
         <v>11.7</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="G85" s="6">
+        <v>4401.2</v>
+      </c>
+      <c r="H85" s="5">
+        <v>2612.6999999999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2482,8 +3000,14 @@
       <c r="F86" s="5">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="G86" s="6">
+        <v>4490.6000000000004</v>
+      </c>
+      <c r="H86" s="5">
+        <v>2674.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2496,8 +3020,14 @@
       <c r="F87" s="5">
         <v>11.7</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="G87" s="6">
+        <v>4566.3999999999996</v>
+      </c>
+      <c r="H87" s="5">
+        <v>2715.6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2510,8 +3040,14 @@
       <c r="F88" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="G88" s="6">
+        <v>4599.3</v>
+      </c>
+      <c r="H88" s="5">
+        <v>2766.6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2527,8 +3063,14 @@
       <c r="F89" s="5">
         <v>12.1</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="G89" s="6">
+        <v>4619.8</v>
+      </c>
+      <c r="H89" s="5">
+        <v>2779.1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2544,8 +3086,14 @@
       <c r="F90" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="G90" s="6">
+        <v>4691.6000000000004</v>
+      </c>
+      <c r="H90" s="5">
+        <v>2810.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2561,8 +3109,14 @@
       <c r="F91" s="5">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="G91" s="6">
+        <v>4706.7</v>
+      </c>
+      <c r="H91" s="5">
+        <v>2828.2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2578,8 +3132,14 @@
       <c r="F92" s="5">
         <v>15.2</v>
       </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="G92" s="6">
+        <v>4736.1000000000004</v>
+      </c>
+      <c r="H92" s="5">
+        <v>2841.9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2595,8 +3155,14 @@
       <c r="F93" s="5">
         <v>16</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="G93" s="6">
+        <v>4715.5</v>
+      </c>
+      <c r="H93" s="5">
+        <v>2864.6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -2612,8 +3178,14 @@
       <c r="F94" s="5">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="G94" s="6">
+        <v>4707.1000000000004</v>
+      </c>
+      <c r="H94" s="5">
+        <v>2882.3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -2629,8 +3201,14 @@
       <c r="F95" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="G95" s="6">
+        <v>4715.3999999999996</v>
+      </c>
+      <c r="H95" s="5">
+        <v>2895.6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -2646,8 +3224,14 @@
       <c r="F96" s="5">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:6">
+      <c r="G96" s="6">
+        <v>4757.2</v>
+      </c>
+      <c r="H96" s="5">
+        <v>2921.1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -2663,8 +3247,14 @@
       <c r="F97" s="5">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="G97" s="6">
+        <v>4708.3</v>
+      </c>
+      <c r="H97" s="5">
+        <v>2913.1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -2680,8 +3270,14 @@
       <c r="F98" s="5">
         <v>16.2</v>
       </c>
-    </row>
-    <row r="99" spans="1:6">
+      <c r="G98" s="6">
+        <v>4834.3</v>
+      </c>
+      <c r="H98" s="5">
+        <v>2968.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -2697,8 +3293,14 @@
       <c r="F99" s="5">
         <v>17.3</v>
       </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="G99" s="6">
+        <v>4861.8999999999996</v>
+      </c>
+      <c r="H99" s="5">
+        <v>2996.1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -2714,8 +3316,14 @@
       <c r="F100" s="5">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="G100" s="6">
+        <v>4900</v>
+      </c>
+      <c r="H100" s="5">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -2731,8 +3339,14 @@
       <c r="F101" s="5">
         <v>18.3</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="G101" s="6">
+        <v>4914.3</v>
+      </c>
+      <c r="H101" s="5">
+        <v>3070.2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2748,8 +3362,14 @@
       <c r="F102" s="5">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="G102" s="6">
+        <v>5002.3999999999996</v>
+      </c>
+      <c r="H102" s="5">
+        <v>3110.8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -2765,8 +3385,14 @@
       <c r="F103" s="5">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="G103" s="6">
+        <v>5118.3</v>
+      </c>
+      <c r="H103" s="5">
+        <v>3170.2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -2782,8 +3408,14 @@
       <c r="F104" s="5">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="G104" s="6">
+        <v>5165.3999999999996</v>
+      </c>
+      <c r="H104" s="5">
+        <v>3219.1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -2799,8 +3431,14 @@
       <c r="F105" s="5">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="G105" s="6">
+        <v>5251.2</v>
+      </c>
+      <c r="H105" s="5">
+        <v>3294.6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -2816,8 +3454,14 @@
       <c r="F106" s="5">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="107" spans="1:6">
+      <c r="G106" s="6">
+        <v>5380.5</v>
+      </c>
+      <c r="H106" s="5">
+        <v>3354.8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -2833,8 +3477,14 @@
       <c r="F107" s="5">
         <v>22.7</v>
       </c>
-    </row>
-    <row r="108" spans="1:6">
+      <c r="G107" s="6">
+        <v>5441.5</v>
+      </c>
+      <c r="H107" s="5">
+        <v>3353.4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2850,8 +3500,14 @@
       <c r="F108" s="5">
         <v>23.4</v>
       </c>
-    </row>
-    <row r="109" spans="1:6">
+      <c r="G108" s="6">
+        <v>5411.9</v>
+      </c>
+      <c r="H108" s="5">
+        <v>3365.3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -2867,8 +3523,14 @@
       <c r="F109" s="5">
         <v>24.7</v>
       </c>
-    </row>
-    <row r="110" spans="1:6">
+      <c r="G109" s="6">
+        <v>5462.4</v>
+      </c>
+      <c r="H109" s="5">
+        <v>3355.5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2884,8 +3546,14 @@
       <c r="F110" s="5">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="111" spans="1:6">
+      <c r="G110" s="6">
+        <v>5417</v>
+      </c>
+      <c r="H110" s="5">
+        <v>3326.2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2901,8 +3569,14 @@
       <c r="F111" s="5">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="112" spans="1:6">
+      <c r="G111" s="6">
+        <v>5431.3</v>
+      </c>
+      <c r="H111" s="5">
+        <v>3337.9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -2918,8 +3592,14 @@
       <c r="F112" s="5">
         <v>27.9</v>
       </c>
-    </row>
-    <row r="113" spans="1:6">
+      <c r="G112" s="6">
+        <v>5378.7</v>
+      </c>
+      <c r="H112" s="5">
+        <v>3351.6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -2935,8 +3615,14 @@
       <c r="F113" s="5">
         <v>29.3</v>
       </c>
-    </row>
-    <row r="114" spans="1:6">
+      <c r="G113" s="6">
+        <v>5357.2</v>
+      </c>
+      <c r="H113" s="5">
+        <v>3302.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -2952,8 +3638,14 @@
       <c r="F114" s="5">
         <v>29.1</v>
       </c>
-    </row>
-    <row r="115" spans="1:6">
+      <c r="G114" s="6">
+        <v>5292.4</v>
+      </c>
+      <c r="H114" s="5">
+        <v>3330.1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -2969,8 +3661,14 @@
       <c r="F115" s="5">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="116" spans="1:6">
+      <c r="G115" s="6">
+        <v>5333.2</v>
+      </c>
+      <c r="H115" s="5">
+        <v>3385.7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -2986,8 +3684,14 @@
       <c r="F116" s="5">
         <v>28.2</v>
       </c>
-    </row>
-    <row r="117" spans="1:6">
+      <c r="G116" s="6">
+        <v>5421.4</v>
+      </c>
+      <c r="H116" s="5">
+        <v>3434.1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -3003,8 +3707,14 @@
       <c r="F117" s="5">
         <v>28.4</v>
       </c>
-    </row>
-    <row r="118" spans="1:6">
+      <c r="G117" s="6">
+        <v>5494.4</v>
+      </c>
+      <c r="H117" s="5">
+        <v>3470.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -3020,8 +3730,14 @@
       <c r="F118" s="5">
         <v>29.4</v>
       </c>
-    </row>
-    <row r="119" spans="1:6">
+      <c r="G118" s="6">
+        <v>5618.5</v>
+      </c>
+      <c r="H118" s="5">
+        <v>3539.9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -3037,8 +3753,14 @@
       <c r="F119" s="5">
         <v>31.6</v>
       </c>
-    </row>
-    <row r="120" spans="1:6">
+      <c r="G119" s="6">
+        <v>5661</v>
+      </c>
+      <c r="H119" s="5">
+        <v>3572.4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -3054,8 +3776,14 @@
       <c r="F120" s="5">
         <v>33.700000000000003</v>
       </c>
-    </row>
-    <row r="121" spans="1:6">
+      <c r="G120" s="6">
+        <v>5689.8</v>
+      </c>
+      <c r="H120" s="5">
+        <v>3610.3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -3071,8 +3799,14 @@
       <c r="F121" s="5">
         <v>36.200000000000003</v>
       </c>
-    </row>
-    <row r="122" spans="1:6">
+      <c r="G121" s="6">
+        <v>5732.5</v>
+      </c>
+      <c r="H121" s="5">
+        <v>3657.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -3088,8 +3822,14 @@
       <c r="F122" s="5">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="123" spans="1:6">
+      <c r="G122" s="6">
+        <v>5799.2</v>
+      </c>
+      <c r="H122" s="5">
+        <v>3699.3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -3105,8 +3845,14 @@
       <c r="F123" s="5">
         <v>38.6</v>
       </c>
-    </row>
-    <row r="124" spans="1:6">
+      <c r="G123" s="6">
+        <v>5913</v>
+      </c>
+      <c r="H123" s="5">
+        <v>3719.7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -3122,8 +3868,14 @@
       <c r="F124" s="5">
         <v>39.6</v>
       </c>
-    </row>
-    <row r="125" spans="1:6">
+      <c r="G124" s="6">
+        <v>6017.6</v>
+      </c>
+      <c r="H124" s="5">
+        <v>3755.2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -3139,8 +3891,14 @@
       <c r="F125" s="5">
         <v>41.6</v>
       </c>
-    </row>
-    <row r="126" spans="1:6">
+      <c r="G125" s="6">
+        <v>6018.2</v>
+      </c>
+      <c r="H125" s="5">
+        <v>3811.8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -3159,8 +3917,14 @@
       <c r="F126" s="5">
         <v>43.7</v>
       </c>
-    </row>
-    <row r="127" spans="1:6">
+      <c r="G126" s="6">
+        <v>6039.2</v>
+      </c>
+      <c r="H126" s="5">
+        <v>3833.8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -3179,8 +3943,14 @@
       <c r="F127" s="5">
         <v>47.8</v>
       </c>
-    </row>
-    <row r="128" spans="1:6">
+      <c r="G127" s="6">
+        <v>6274</v>
+      </c>
+      <c r="H127" s="5">
+        <v>3915.6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -3199,8 +3969,14 @@
       <c r="F128" s="5">
         <v>50.4</v>
       </c>
-    </row>
-    <row r="129" spans="1:6">
+      <c r="G128" s="6">
+        <v>6335.3</v>
+      </c>
+      <c r="H128" s="5">
+        <v>3932</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -3219,8 +3995,14 @@
       <c r="F129" s="5">
         <v>52.9</v>
       </c>
-    </row>
-    <row r="130" spans="1:6">
+      <c r="G129" s="6">
+        <v>6420.3</v>
+      </c>
+      <c r="H129" s="5">
+        <v>3963.5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -3239,8 +4021,14 @@
       <c r="F130" s="5">
         <v>55.5</v>
       </c>
-    </row>
-    <row r="131" spans="1:6">
+      <c r="G130" s="6">
+        <v>6433</v>
+      </c>
+      <c r="H130" s="5">
+        <v>3983.6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -3259,8 +4047,14 @@
       <c r="F131" s="5">
         <v>56.7</v>
       </c>
-    </row>
-    <row r="132" spans="1:6">
+      <c r="G131" s="6">
+        <v>6440.8</v>
+      </c>
+      <c r="H131" s="5">
+        <v>3981.3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -3279,8 +4073,14 @@
       <c r="F132" s="5">
         <v>59.4</v>
       </c>
-    </row>
-    <row r="133" spans="1:6">
+      <c r="G132" s="6">
+        <v>6487.1</v>
+      </c>
+      <c r="H132" s="5">
+        <v>4020.4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -3299,8 +4099,14 @@
       <c r="F133" s="5">
         <v>62.3</v>
       </c>
-    </row>
-    <row r="134" spans="1:6">
+      <c r="G133" s="6">
+        <v>6503.9</v>
+      </c>
+      <c r="H133" s="5">
+        <v>4031.2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -3319,8 +4125,14 @@
       <c r="F134" s="5">
         <v>65.400000000000006</v>
       </c>
-    </row>
-    <row r="135" spans="1:6">
+      <c r="G134" s="6">
+        <v>6524.9</v>
+      </c>
+      <c r="H134" s="5">
+        <v>4025</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -3339,8 +4151,14 @@
       <c r="F135" s="5">
         <v>66.7</v>
       </c>
-    </row>
-    <row r="136" spans="1:6">
+      <c r="G135" s="6">
+        <v>6392.6</v>
+      </c>
+      <c r="H135" s="5">
+        <v>3934.5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -3359,8 +4177,14 @@
       <c r="F136" s="5">
         <v>70.7</v>
       </c>
-    </row>
-    <row r="137" spans="1:6">
+      <c r="G136" s="6">
+        <v>6382.9</v>
+      </c>
+      <c r="H136" s="5">
+        <v>3976.9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -3379,8 +4203,14 @@
       <c r="F137" s="5">
         <v>72.3</v>
       </c>
-    </row>
-    <row r="138" spans="1:6">
+      <c r="G137" s="6">
+        <v>6501.2</v>
+      </c>
+      <c r="H137" s="5">
+        <v>4029.6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -3399,8 +4229,14 @@
       <c r="F138" s="5">
         <v>76.5</v>
       </c>
-    </row>
-    <row r="139" spans="1:6">
+      <c r="G138" s="6">
+        <v>6635.7</v>
+      </c>
+      <c r="H138" s="5">
+        <v>4050.8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -3419,8 +4255,14 @@
       <c r="F139" s="5">
         <v>79.5</v>
       </c>
-    </row>
-    <row r="140" spans="1:6">
+      <c r="G139" s="6">
+        <v>6587.3</v>
+      </c>
+      <c r="H139" s="5">
+        <v>4050.1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -3439,8 +4281,14 @@
       <c r="F140" s="5">
         <v>82.9</v>
       </c>
-    </row>
-    <row r="141" spans="1:6">
+      <c r="G140" s="6">
+        <v>6662.9</v>
+      </c>
+      <c r="H140" s="5">
+        <v>4066.4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -3459,8 +4307,14 @@
       <c r="F141" s="5">
         <v>87</v>
       </c>
-    </row>
-    <row r="142" spans="1:6">
+      <c r="G141" s="6">
+        <v>6585.1</v>
+      </c>
+      <c r="H141" s="5">
+        <v>4035.9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -3479,8 +4333,14 @@
       <c r="F142" s="5">
         <v>90.2</v>
       </c>
-    </row>
-    <row r="143" spans="1:6">
+      <c r="G142" s="6">
+        <v>6475</v>
+      </c>
+      <c r="H142" s="5">
+        <v>4062.6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -3499,8 +4359,14 @@
       <c r="F143" s="5">
         <v>87.5</v>
       </c>
-    </row>
-    <row r="144" spans="1:6">
+      <c r="G143" s="6">
+        <v>6510.2</v>
+      </c>
+      <c r="H143" s="5">
+        <v>4077.6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -3519,8 +4385,14 @@
       <c r="F144" s="5">
         <v>88.4</v>
       </c>
-    </row>
-    <row r="145" spans="1:6">
+      <c r="G144" s="6">
+        <v>6486.8</v>
+      </c>
+      <c r="H144" s="5">
+        <v>4109.1000000000004</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -3539,8 +4411,14 @@
       <c r="F145" s="5">
         <v>86.9</v>
       </c>
-    </row>
-    <row r="146" spans="1:6">
+      <c r="G145" s="6">
+        <v>6493.1</v>
+      </c>
+      <c r="H145" s="5">
+        <v>4184.1000000000004</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -3559,8 +4437,14 @@
       <c r="F146" s="5">
         <v>92.1</v>
       </c>
-    </row>
-    <row r="147" spans="1:6">
+      <c r="G146" s="6">
+        <v>6578.2</v>
+      </c>
+      <c r="H146" s="5">
+        <v>4224.8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -3579,8 +4463,14 @@
       <c r="F147" s="5">
         <v>97.4</v>
       </c>
-    </row>
-    <row r="148" spans="1:6">
+      <c r="G147" s="6">
+        <v>6728.3</v>
+      </c>
+      <c r="H147" s="5">
+        <v>4308.3999999999996</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -3599,8 +4489,14 @@
       <c r="F148" s="5">
         <v>101.3</v>
       </c>
-    </row>
-    <row r="149" spans="1:6">
+      <c r="G148" s="6">
+        <v>6860</v>
+      </c>
+      <c r="H148" s="5">
+        <v>4384</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -3619,8 +4515,14 @@
       <c r="F149" s="5">
         <v>109.5</v>
       </c>
-    </row>
-    <row r="150" spans="1:6">
+      <c r="G149" s="6">
+        <v>7001.5</v>
+      </c>
+      <c r="H149" s="5">
+        <v>4453.1000000000004</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -3639,8 +4541,14 @@
       <c r="F150" s="5">
         <v>112</v>
       </c>
-    </row>
-    <row r="151" spans="1:6">
+      <c r="G150" s="6">
+        <v>7140.6</v>
+      </c>
+      <c r="H150" s="5">
+        <v>4490.8999999999996</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -3659,8 +4567,14 @@
       <c r="F151" s="5">
         <v>119.2</v>
       </c>
-    </row>
-    <row r="152" spans="1:6">
+      <c r="G151" s="6">
+        <v>7266</v>
+      </c>
+      <c r="H151" s="5">
+        <v>4554.8999999999996</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -3679,8 +4593,14 @@
       <c r="F152" s="5">
         <v>124.2</v>
       </c>
-    </row>
-    <row r="153" spans="1:6">
+      <c r="G152" s="6">
+        <v>7337.5</v>
+      </c>
+      <c r="H152" s="5">
+        <v>4589.8999999999996</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -3699,8 +4619,14 @@
       <c r="F153" s="5">
         <v>130.69999999999999</v>
       </c>
-    </row>
-    <row r="154" spans="1:6">
+      <c r="G153" s="6">
+        <v>7396</v>
+      </c>
+      <c r="H153" s="5">
+        <v>4650.6000000000004</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -3719,8 +4645,14 @@
       <c r="F154" s="5">
         <v>128.9</v>
       </c>
-    </row>
-    <row r="155" spans="1:6">
+      <c r="G154" s="6">
+        <v>7469.5</v>
+      </c>
+      <c r="H154" s="5">
+        <v>4729.7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -3739,8 +4671,14 @@
       <c r="F155" s="5">
         <v>131.4</v>
       </c>
-    </row>
-    <row r="156" spans="1:6">
+      <c r="G155" s="6">
+        <v>7537.9</v>
+      </c>
+      <c r="H155" s="5">
+        <v>4774.1000000000004</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -3759,8 +4697,14 @@
       <c r="F156" s="5">
         <v>128.69999999999999</v>
       </c>
-    </row>
-    <row r="157" spans="1:6">
+      <c r="G156" s="6">
+        <v>7655.2</v>
+      </c>
+      <c r="H156" s="5">
+        <v>4865.8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -3779,8 +4723,14 @@
       <c r="F157" s="5">
         <v>132.5</v>
       </c>
-    </row>
-    <row r="158" spans="1:6">
+      <c r="G157" s="6">
+        <v>7712.6</v>
+      </c>
+      <c r="H157" s="5">
+        <v>4878.3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -3799,8 +4749,14 @@
       <c r="F158" s="5">
         <v>133</v>
       </c>
-    </row>
-    <row r="159" spans="1:6">
+      <c r="G158" s="6">
+        <v>7784.1</v>
+      </c>
+      <c r="H158" s="5">
+        <v>4919.6000000000004</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -3819,8 +4775,14 @@
       <c r="F159" s="5">
         <v>136.5</v>
       </c>
-    </row>
-    <row r="160" spans="1:6">
+      <c r="G159" s="6">
+        <v>7819.8</v>
+      </c>
+      <c r="H159" s="5">
+        <v>4974.6000000000004</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -3839,8 +4801,14 @@
       <c r="F160" s="5">
         <v>136.30000000000001</v>
       </c>
-    </row>
-    <row r="161" spans="1:6">
+      <c r="G160" s="6">
+        <v>7898.6</v>
+      </c>
+      <c r="H160" s="5">
+        <v>5064.7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -3859,8 +4827,14 @@
       <c r="F161" s="5">
         <v>141.30000000000001</v>
       </c>
-    </row>
-    <row r="162" spans="1:6">
+      <c r="G161" s="6">
+        <v>7939.5</v>
+      </c>
+      <c r="H161" s="5">
+        <v>5097.1000000000004</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -3879,8 +4853,14 @@
       <c r="F162" s="5">
         <v>137.6</v>
       </c>
-    </row>
-    <row r="163" spans="1:6">
+      <c r="G162" s="6">
+        <v>7995</v>
+      </c>
+      <c r="H162" s="5">
+        <v>5097.8999999999996</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -3899,8 +4879,14 @@
       <c r="F163" s="5">
         <v>138.9</v>
       </c>
-    </row>
-    <row r="164" spans="1:6">
+      <c r="G163" s="6">
+        <v>8084.7</v>
+      </c>
+      <c r="H163" s="5">
+        <v>5168.6000000000004</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -3919,8 +4905,14 @@
       <c r="F164" s="5">
         <v>143.6</v>
       </c>
-    </row>
-    <row r="165" spans="1:6">
+      <c r="G164" s="6">
+        <v>8158</v>
+      </c>
+      <c r="H164" s="5">
+        <v>5228.5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -3939,8 +4931,14 @@
       <c r="F165" s="5">
         <v>144.6</v>
       </c>
-    </row>
-    <row r="166" spans="1:6">
+      <c r="G165" s="6">
+        <v>8292.7000000000007</v>
+      </c>
+      <c r="H165" s="5">
+        <v>5239.5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -3959,8 +4957,14 @@
       <c r="F166" s="5">
         <v>148.9</v>
       </c>
-    </row>
-    <row r="167" spans="1:6">
+      <c r="G166" s="6">
+        <v>8339.2999999999993</v>
+      </c>
+      <c r="H166" s="5">
+        <v>5332.7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -3979,8 +4983,14 @@
       <c r="F167" s="5">
         <v>154.30000000000001</v>
       </c>
-    </row>
-    <row r="168" spans="1:6">
+      <c r="G167" s="6">
+        <v>8449.5</v>
+      </c>
+      <c r="H167" s="5">
+        <v>5371.8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -3999,8 +5009,14 @@
       <c r="F168" s="5">
         <v>156.9</v>
       </c>
-    </row>
-    <row r="169" spans="1:6">
+      <c r="G168" s="6">
+        <v>8498.2999999999993</v>
+      </c>
+      <c r="H168" s="5">
+        <v>5417.7</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -4019,8 +5035,14 @@
       <c r="F169" s="5">
         <v>159.69999999999999</v>
       </c>
-    </row>
-    <row r="170" spans="1:6">
+      <c r="G169" s="6">
+        <v>8610.9</v>
+      </c>
+      <c r="H169" s="5">
+        <v>5479.7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -4039,8 +5061,14 @@
       <c r="F170" s="5">
         <v>164.9</v>
       </c>
-    </row>
-    <row r="171" spans="1:6">
+      <c r="G170" s="6">
+        <v>8697.7000000000007</v>
+      </c>
+      <c r="H170" s="5">
+        <v>5505</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -4059,8 +5087,14 @@
       <c r="F171" s="5">
         <v>171.7</v>
       </c>
-    </row>
-    <row r="172" spans="1:6">
+      <c r="G171" s="6">
+        <v>8766.1</v>
+      </c>
+      <c r="H171" s="5">
+        <v>5530.9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -4079,8 +5113,14 @@
       <c r="F172" s="5">
         <v>176.3</v>
       </c>
-    </row>
-    <row r="173" spans="1:6">
+      <c r="G172" s="6">
+        <v>8831.5</v>
+      </c>
+      <c r="H172" s="5">
+        <v>5585.9</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -4099,8 +5139,14 @@
       <c r="F173" s="5">
         <v>177.4</v>
       </c>
-    </row>
-    <row r="174" spans="1:6">
+      <c r="G173" s="6">
+        <v>8850.2000000000007</v>
+      </c>
+      <c r="H173" s="5">
+        <v>5610.5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -4119,8 +5165,14 @@
       <c r="F174" s="5">
         <v>178.4</v>
       </c>
-    </row>
-    <row r="175" spans="1:6">
+      <c r="G174" s="6">
+        <v>8947.1</v>
+      </c>
+      <c r="H174" s="5">
+        <v>5658.7</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -4139,8 +5191,14 @@
       <c r="F175" s="5">
         <v>176.7</v>
       </c>
-    </row>
-    <row r="176" spans="1:6">
+      <c r="G175" s="6">
+        <v>8981.7000000000007</v>
+      </c>
+      <c r="H175" s="5">
+        <v>5676.4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -4159,8 +5217,14 @@
       <c r="F176" s="5">
         <v>174.6</v>
       </c>
-    </row>
-    <row r="177" spans="1:6">
+      <c r="G176" s="6">
+        <v>8983.9</v>
+      </c>
+      <c r="H176" s="5">
+        <v>5699.3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -4179,8 +5243,14 @@
       <c r="F177" s="5">
         <v>179</v>
       </c>
-    </row>
-    <row r="178" spans="1:6">
+      <c r="G177" s="6">
+        <v>8907.4</v>
+      </c>
+      <c r="H177" s="5">
+        <v>5656.2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -4199,8 +5269,14 @@
       <c r="F178" s="5">
         <v>177.6</v>
       </c>
-    </row>
-    <row r="179" spans="1:6">
+      <c r="G178" s="6">
+        <v>8865.6</v>
+      </c>
+      <c r="H178" s="5">
+        <v>5636.7</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -4219,8 +5295,14 @@
       <c r="F179" s="5">
         <v>181.1</v>
       </c>
-    </row>
-    <row r="180" spans="1:6">
+      <c r="G179" s="6">
+        <v>8934.4</v>
+      </c>
+      <c r="H179" s="5">
+        <v>5684</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -4239,8 +5321,14 @@
       <c r="F180" s="5">
         <v>184.5</v>
       </c>
-    </row>
-    <row r="181" spans="1:6">
+      <c r="G180" s="6">
+        <v>8977.2999999999993</v>
+      </c>
+      <c r="H180" s="5">
+        <v>5711.6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -4259,8 +5347,14 @@
       <c r="F181" s="5">
         <v>188.5</v>
       </c>
-    </row>
-    <row r="182" spans="1:6">
+      <c r="G181" s="6">
+        <v>9016.4</v>
+      </c>
+      <c r="H181" s="5">
+        <v>5710.1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -4279,8 +5373,14 @@
       <c r="F182" s="5">
         <v>190.2</v>
       </c>
-    </row>
-    <row r="183" spans="1:6">
+      <c r="G182" s="6">
+        <v>9123</v>
+      </c>
+      <c r="H182" s="5">
+        <v>5817.3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -4299,8 +5399,14 @@
       <c r="F183" s="5">
         <v>197.3</v>
       </c>
-    </row>
-    <row r="184" spans="1:6">
+      <c r="G183" s="6">
+        <v>9223.5</v>
+      </c>
+      <c r="H183" s="5">
+        <v>5857.2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -4319,8 +5425,14 @@
       <c r="F184" s="5">
         <v>205.6</v>
       </c>
-    </row>
-    <row r="185" spans="1:6">
+      <c r="G184" s="6">
+        <v>9313.2000000000007</v>
+      </c>
+      <c r="H184" s="5">
+        <v>5920.6</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -4339,8 +5451,14 @@
       <c r="F185" s="5">
         <v>206.6</v>
       </c>
-    </row>
-    <row r="186" spans="1:6">
+      <c r="G185" s="6">
+        <v>9406.5</v>
+      </c>
+      <c r="H185" s="5">
+        <v>5991.1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -4359,8 +5477,14 @@
       <c r="F186" s="5">
         <v>211.3</v>
       </c>
-    </row>
-    <row r="187" spans="1:6">
+      <c r="G186" s="6">
+        <v>9424.1</v>
+      </c>
+      <c r="H186" s="5">
+        <v>6013.8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -4379,8 +5503,14 @@
       <c r="F187" s="5">
         <v>213.3</v>
       </c>
-    </row>
-    <row r="188" spans="1:6">
+      <c r="G187" s="6">
+        <v>9480.1</v>
+      </c>
+      <c r="H187" s="5">
+        <v>6067.8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -4399,8 +5529,14 @@
       <c r="F188" s="5">
         <v>222.1</v>
       </c>
-    </row>
-    <row r="189" spans="1:6">
+      <c r="G188" s="6">
+        <v>9526.2999999999993</v>
+      </c>
+      <c r="H188" s="5">
+        <v>6134.8</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -4419,8 +5555,14 @@
       <c r="F189" s="5">
         <v>223.6</v>
       </c>
-    </row>
-    <row r="190" spans="1:6">
+      <c r="G189" s="6">
+        <v>9653.5</v>
+      </c>
+      <c r="H189" s="5">
+        <v>6189.1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -4439,8 +5581,14 @@
       <c r="F190" s="5">
         <v>228.8</v>
       </c>
-    </row>
-    <row r="191" spans="1:6">
+      <c r="G190" s="6">
+        <v>9748.2000000000007</v>
+      </c>
+      <c r="H190" s="5">
+        <v>6260.1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -4459,8 +5607,14 @@
       <c r="F191" s="5">
         <v>232.4</v>
       </c>
-    </row>
-    <row r="192" spans="1:6">
+      <c r="G191" s="6">
+        <v>9881.4</v>
+      </c>
+      <c r="H191" s="5">
+        <v>6308.6</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -4479,8 +5633,14 @@
       <c r="F192" s="5">
         <v>236.4</v>
       </c>
-    </row>
-    <row r="193" spans="1:6">
+      <c r="G192" s="6">
+        <v>9939.7000000000007</v>
+      </c>
+      <c r="H192" s="5">
+        <v>6357.5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -4499,8 +5659,14 @@
       <c r="F193" s="5">
         <v>243.3</v>
       </c>
-    </row>
-    <row r="194" spans="1:6">
+      <c r="G193" s="6">
+        <v>10052.5</v>
+      </c>
+      <c r="H193" s="5">
+        <v>6425.9</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -4519,8 +5685,14 @@
       <c r="F194" s="5">
         <v>252.3</v>
       </c>
-    </row>
-    <row r="195" spans="1:6">
+      <c r="G194" s="6">
+        <v>10086.9</v>
+      </c>
+      <c r="H194" s="5">
+        <v>6442.9</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -4539,8 +5711,14 @@
       <c r="F195" s="5">
         <v>262.5</v>
       </c>
-    </row>
-    <row r="196" spans="1:6">
+      <c r="G195" s="6">
+        <v>10122.1</v>
+      </c>
+      <c r="H195" s="5">
+        <v>6500.7</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -4559,8 +5737,14 @@
       <c r="F196" s="5">
         <v>263.7</v>
       </c>
-    </row>
-    <row r="197" spans="1:6">
+      <c r="G196" s="6">
+        <v>10208.799999999999</v>
+      </c>
+      <c r="H196" s="5">
+        <v>6560.3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -4579,8 +5763,14 @@
       <c r="F197" s="5">
         <v>273.5</v>
       </c>
-    </row>
-    <row r="198" spans="1:6">
+      <c r="G197" s="6">
+        <v>10281.200000000001</v>
+      </c>
+      <c r="H197" s="5">
+        <v>6606.4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -4599,8 +5789,14 @@
       <c r="F198" s="5">
         <v>281.5</v>
       </c>
-    </row>
-    <row r="199" spans="1:6">
+      <c r="G198" s="6">
+        <v>10348.700000000001</v>
+      </c>
+      <c r="H198" s="5">
+        <v>6667.7</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -4619,8 +5815,14 @@
       <c r="F199" s="5">
         <v>285.89999999999998</v>
       </c>
-    </row>
-    <row r="200" spans="1:6">
+      <c r="G199" s="6">
+        <v>10529.4</v>
+      </c>
+      <c r="H199" s="5">
+        <v>6740.1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -4639,8 +5841,14 @@
       <c r="F200" s="5">
         <v>294.2</v>
       </c>
-    </row>
-    <row r="201" spans="1:6">
+      <c r="G200" s="6">
+        <v>10626.8</v>
+      </c>
+      <c r="H200" s="5">
+        <v>6780.7</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -4659,8 +5867,14 @@
       <c r="F201" s="5">
         <v>299</v>
       </c>
-    </row>
-    <row r="202" spans="1:6">
+      <c r="G201" s="6">
+        <v>10739.1</v>
+      </c>
+      <c r="H201" s="5">
+        <v>6834</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -4679,8 +5893,14 @@
       <c r="F202" s="5">
         <v>311.5</v>
       </c>
-    </row>
-    <row r="203" spans="1:6">
+      <c r="G202" s="6">
+        <v>10820.9</v>
+      </c>
+      <c r="H202" s="5">
+        <v>6906.1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -4699,8 +5919,14 @@
       <c r="F203" s="5">
         <v>323.2</v>
       </c>
-    </row>
-    <row r="204" spans="1:6">
+      <c r="G203" s="6">
+        <v>10984.2</v>
+      </c>
+      <c r="H203" s="5">
+        <v>6937.4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -4719,8 +5945,14 @@
       <c r="F204" s="5">
         <v>340.6</v>
       </c>
-    </row>
-    <row r="205" spans="1:6">
+      <c r="G204" s="6">
+        <v>11124</v>
+      </c>
+      <c r="H204" s="5">
+        <v>7056.1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -4739,8 +5971,14 @@
       <c r="F205" s="5">
         <v>345.9</v>
       </c>
-    </row>
-    <row r="206" spans="1:6">
+      <c r="G205" s="6">
+        <v>11210.3</v>
+      </c>
+      <c r="H205" s="5">
+        <v>7139.9</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -4759,8 +5997,14 @@
       <c r="F206" s="5">
         <v>357.1</v>
       </c>
-    </row>
-    <row r="207" spans="1:6">
+      <c r="G206" s="6">
+        <v>11321.2</v>
+      </c>
+      <c r="H206" s="5">
+        <v>7213.6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -4779,8 +6023,14 @@
       <c r="F207" s="5">
         <v>362.5</v>
       </c>
-    </row>
-    <row r="208" spans="1:6">
+      <c r="G207" s="6">
+        <v>11431</v>
+      </c>
+      <c r="H207" s="5">
+        <v>7341</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -4799,8 +6049,14 @@
       <c r="F208" s="5">
         <v>365.7</v>
       </c>
-    </row>
-    <row r="209" spans="1:6">
+      <c r="G208" s="6">
+        <v>11580.6</v>
+      </c>
+      <c r="H208" s="5">
+        <v>7437.5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -4819,8 +6075,14 @@
       <c r="F209" s="5">
         <v>379.1</v>
       </c>
-    </row>
-    <row r="210" spans="1:6">
+      <c r="G209" s="6">
+        <v>11770.7</v>
+      </c>
+      <c r="H209" s="5">
+        <v>7546.8</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -4839,8 +6101,14 @@
       <c r="F210" s="5">
         <v>393.6</v>
       </c>
-    </row>
-    <row r="211" spans="1:6">
+      <c r="G210" s="6">
+        <v>11864.7</v>
+      </c>
+      <c r="H210" s="5">
+        <v>7618.7</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -4859,8 +6127,14 @@
       <c r="F211" s="5">
         <v>416.2</v>
       </c>
-    </row>
-    <row r="212" spans="1:6">
+      <c r="G211" s="6">
+        <v>11962.5</v>
+      </c>
+      <c r="H211" s="5">
+        <v>7731.5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -4879,8 +6153,14 @@
       <c r="F212" s="5">
         <v>429.5</v>
       </c>
-    </row>
-    <row r="213" spans="1:6">
+      <c r="G212" s="6">
+        <v>12113.1</v>
+      </c>
+      <c r="H212" s="5">
+        <v>7819.3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -4899,8 +6179,14 @@
       <c r="F213" s="5">
         <v>429</v>
       </c>
-    </row>
-    <row r="214" spans="1:6">
+      <c r="G213" s="6">
+        <v>12323.3</v>
+      </c>
+      <c r="H213" s="5">
+        <v>7934.1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -4919,8 +6205,14 @@
       <c r="F214" s="5">
         <v>455.7</v>
       </c>
-    </row>
-    <row r="215" spans="1:6">
+      <c r="G214" s="6">
+        <v>12359.1</v>
+      </c>
+      <c r="H214" s="5">
+        <v>8054.9</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -4939,8 +6231,14 @@
       <c r="F215" s="5">
         <v>476.6</v>
       </c>
-    </row>
-    <row r="216" spans="1:6">
+      <c r="G215" s="6">
+        <v>12592.5</v>
+      </c>
+      <c r="H215" s="5">
+        <v>8132.2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -4959,8 +6257,14 @@
       <c r="F216" s="5">
         <v>484.6</v>
       </c>
-    </row>
-    <row r="217" spans="1:6">
+      <c r="G216" s="6">
+        <v>12607.7</v>
+      </c>
+      <c r="H216" s="5">
+        <v>8211.2999999999993</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -4979,8 +6283,14 @@
       <c r="F217" s="5">
         <v>496</v>
       </c>
-    </row>
-    <row r="218" spans="1:6">
+      <c r="G217" s="6">
+        <v>12679.3</v>
+      </c>
+      <c r="H217" s="5">
+        <v>8284.4</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -4999,8 +6309,14 @@
       <c r="F218" s="5">
         <v>484.3</v>
       </c>
-    </row>
-    <row r="219" spans="1:6">
+      <c r="G218" s="6">
+        <v>12643.3</v>
+      </c>
+      <c r="H218" s="5">
+        <v>8319.4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -5019,8 +6335,14 @@
       <c r="F219" s="5">
         <v>459.1</v>
       </c>
-    </row>
-    <row r="220" spans="1:6">
+      <c r="G219" s="6">
+        <v>12710.3</v>
+      </c>
+      <c r="H219" s="5">
+        <v>8340.7999999999993</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -5039,8 +6361,14 @@
       <c r="F220" s="5">
         <v>438.4</v>
       </c>
-    </row>
-    <row r="221" spans="1:6">
+      <c r="G220" s="6">
+        <v>12670.1</v>
+      </c>
+      <c r="H220" s="5">
+        <v>8371.2000000000007</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -5059,8 +6387,14 @@
       <c r="F221" s="5">
         <v>428.3</v>
       </c>
-    </row>
-    <row r="222" spans="1:6">
+      <c r="G221" s="6">
+        <v>12705.3</v>
+      </c>
+      <c r="H221" s="5">
+        <v>8499.1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -5079,8 +6413,14 @@
       <c r="F222" s="5">
         <v>422.1</v>
       </c>
-    </row>
-    <row r="223" spans="1:6">
+      <c r="G222" s="6">
+        <v>12822.3</v>
+      </c>
+      <c r="H222" s="5">
+        <v>8524.6</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -5099,8 +6439,14 @@
       <c r="F223" s="5">
         <v>420.5</v>
       </c>
-    </row>
-    <row r="224" spans="1:6">
+      <c r="G223" s="6">
+        <v>12893</v>
+      </c>
+      <c r="H223" s="5">
+        <v>8568.1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -5119,8 +6465,14 @@
       <c r="F224" s="5">
         <v>424.9</v>
       </c>
-    </row>
-    <row r="225" spans="1:6">
+      <c r="G224" s="6">
+        <v>12955.8</v>
+      </c>
+      <c r="H224" s="5">
+        <v>8628</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -5139,8 +6491,14 @@
       <c r="F225" s="5">
         <v>411.6</v>
       </c>
-    </row>
-    <row r="226" spans="1:6">
+      <c r="G225" s="6">
+        <v>12964</v>
+      </c>
+      <c r="H225" s="5">
+        <v>8674.4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -5159,8 +6517,14 @@
       <c r="F226" s="5">
         <v>417.4</v>
       </c>
-    </row>
-    <row r="227" spans="1:6">
+      <c r="G226" s="6">
+        <v>13031.2</v>
+      </c>
+      <c r="H226" s="5">
+        <v>8712.5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -5179,8 +6543,14 @@
       <c r="F227" s="5">
         <v>420.4</v>
       </c>
-    </row>
-    <row r="228" spans="1:6">
+      <c r="G227" s="6">
+        <v>13152.1</v>
+      </c>
+      <c r="H227" s="5">
+        <v>8809.5</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -5199,8 +6569,14 @@
       <c r="F228" s="5">
         <v>438.6</v>
       </c>
-    </row>
-    <row r="229" spans="1:6">
+      <c r="G228" s="6">
+        <v>13372.4</v>
+      </c>
+      <c r="H228" s="5">
+        <v>8939.4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -5219,8 +6595,14 @@
       <c r="F229" s="5">
         <v>451.7</v>
       </c>
-    </row>
-    <row r="230" spans="1:6">
+      <c r="G229" s="6">
+        <v>13528.7</v>
+      </c>
+      <c r="H229" s="5">
+        <v>9008.7999999999993</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -5239,8 +6621,14 @@
       <c r="F230" s="5">
         <v>449.8</v>
       </c>
-    </row>
-    <row r="231" spans="1:6">
+      <c r="G230" s="6">
+        <v>13606.5</v>
+      </c>
+      <c r="H230" s="5">
+        <v>9096.4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -5259,8 +6647,14 @@
       <c r="F231" s="5">
         <v>455.1</v>
       </c>
-    </row>
-    <row r="232" spans="1:6">
+      <c r="G231" s="6">
+        <v>13706.2</v>
+      </c>
+      <c r="H231" s="5">
+        <v>9155.5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -5279,8 +6673,14 @@
       <c r="F232" s="5">
         <v>461.4</v>
       </c>
-    </row>
-    <row r="233" spans="1:6">
+      <c r="G232" s="6">
+        <v>13830.8</v>
+      </c>
+      <c r="H232" s="5">
+        <v>9243</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -5299,8 +6699,14 @@
       <c r="F233" s="5">
         <v>466.4</v>
       </c>
-    </row>
-    <row r="234" spans="1:6">
+      <c r="G233" s="6">
+        <v>13950.4</v>
+      </c>
+      <c r="H233" s="5">
+        <v>9337.7999999999993</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -5319,8 +6725,14 @@
       <c r="F234" s="5">
         <v>471.3</v>
       </c>
-    </row>
-    <row r="235" spans="1:6">
+      <c r="G234" s="6">
+        <v>14099.1</v>
+      </c>
+      <c r="H234" s="5">
+        <v>9409.2000000000007</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -5339,8 +6751,14 @@
       <c r="F235" s="5">
         <v>477.6</v>
       </c>
-    </row>
-    <row r="236" spans="1:6">
+      <c r="G235" s="6">
+        <v>14172.7</v>
+      </c>
+      <c r="H235" s="5">
+        <v>9511.5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -5359,8 +6777,14 @@
       <c r="F236" s="5">
         <v>484.8</v>
       </c>
-    </row>
-    <row r="237" spans="1:6">
+      <c r="G236" s="6">
+        <v>14291.8</v>
+      </c>
+      <c r="H236" s="5">
+        <v>9585.2000000000007</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -5379,8 +6803,14 @@
       <c r="F237" s="5">
         <v>486.1</v>
       </c>
-    </row>
-    <row r="238" spans="1:6">
+      <c r="G237" s="6">
+        <v>14373.4</v>
+      </c>
+      <c r="H237" s="5">
+        <v>9621.2999999999993</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -5399,8 +6829,14 @@
       <c r="F238" s="5">
         <v>503.7</v>
       </c>
-    </row>
-    <row r="239" spans="1:6">
+      <c r="G238" s="6">
+        <v>14546.1</v>
+      </c>
+      <c r="H238" s="5">
+        <v>9729.2000000000007</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -5419,8 +6855,14 @@
       <c r="F239" s="5">
         <v>505.9</v>
       </c>
-    </row>
-    <row r="240" spans="1:6">
+      <c r="G239" s="6">
+        <v>14589.6</v>
+      </c>
+      <c r="H239" s="5">
+        <v>9781</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -5439,8 +6881,14 @@
       <c r="F240" s="5">
         <v>516.29999999999995</v>
       </c>
-    </row>
-    <row r="241" spans="1:6">
+      <c r="G240" s="6">
+        <v>14602.6</v>
+      </c>
+      <c r="H240" s="5">
+        <v>9838.1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -5459,8 +6907,14 @@
       <c r="F241" s="5">
         <v>519</v>
       </c>
-    </row>
-    <row r="242" spans="1:6">
+      <c r="G241" s="6">
+        <v>14716.9</v>
+      </c>
+      <c r="H241" s="5">
+        <v>9938.4</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -5479,8 +6933,14 @@
       <c r="F242" s="5">
         <v>541.5</v>
       </c>
-    </row>
-    <row r="243" spans="1:6">
+      <c r="G242" s="6">
+        <v>14726</v>
+      </c>
+      <c r="H242" s="5">
+        <v>9990.7000000000007</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -5499,8 +6959,14 @@
       <c r="F243" s="5">
         <v>542.9</v>
       </c>
-    </row>
-    <row r="244" spans="1:6">
+      <c r="G243" s="6">
+        <v>14838.7</v>
+      </c>
+      <c r="H243" s="5">
+        <v>10024.6</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -5519,8 +6985,14 @@
       <c r="F244" s="5">
         <v>545.4</v>
       </c>
-    </row>
-    <row r="245" spans="1:6">
+      <c r="G244" s="6">
+        <v>14938.5</v>
+      </c>
+      <c r="H244" s="5">
+        <v>10069.200000000001</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -5539,8 +7011,14 @@
       <c r="F245" s="5">
         <v>559.79999999999995</v>
       </c>
-    </row>
-    <row r="246" spans="1:6">
+      <c r="G245" s="6">
+        <v>14991.8</v>
+      </c>
+      <c r="H245" s="5">
+        <v>10081.799999999999</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -5559,8 +7037,14 @@
       <c r="F246" s="5">
         <v>564.70000000000005</v>
       </c>
-    </row>
-    <row r="247" spans="1:6">
+      <c r="G246" s="6">
+        <v>14889.5</v>
+      </c>
+      <c r="H246" s="5">
+        <v>10061</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -5579,8 +7063,14 @@
       <c r="F247" s="5">
         <v>564.9</v>
       </c>
-    </row>
-    <row r="248" spans="1:6">
+      <c r="G247" s="6">
+        <v>14963.4</v>
+      </c>
+      <c r="H247" s="5">
+        <v>10077.9</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -5599,8 +7089,14 @@
       <c r="F248" s="5">
         <v>551.9</v>
       </c>
-    </row>
-    <row r="249" spans="1:6">
+      <c r="G248" s="6">
+        <v>14891.6</v>
+      </c>
+      <c r="H248" s="5">
+        <v>10005.1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -5619,8 +7115,14 @@
       <c r="F249" s="5">
         <v>517.70000000000005</v>
       </c>
-    </row>
-    <row r="250" spans="1:6">
+      <c r="G249" s="6">
+        <v>14577</v>
+      </c>
+      <c r="H249" s="5">
+        <v>9884.7000000000007</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -5639,8 +7141,14 @@
       <c r="F250" s="5">
         <v>503.1</v>
       </c>
-    </row>
-    <row r="251" spans="1:6">
+      <c r="G250" s="6">
+        <v>14375</v>
+      </c>
+      <c r="H250" s="5">
+        <v>9850.7999999999993</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -5659,8 +7167,14 @@
       <c r="F251" s="5">
         <v>501.8</v>
       </c>
-    </row>
-    <row r="252" spans="1:6">
+      <c r="G251" s="6">
+        <v>14355.6</v>
+      </c>
+      <c r="H251" s="5">
+        <v>9806.4</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -5679,8 +7193,14 @@
       <c r="F252" s="5">
         <v>517.4</v>
       </c>
-    </row>
-    <row r="253" spans="1:6">
+      <c r="G252" s="6">
+        <v>14402.5</v>
+      </c>
+      <c r="H252" s="5">
+        <v>9865.9</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -5699,8 +7219,14 @@
       <c r="F253" s="5">
         <v>529.20000000000005</v>
       </c>
-    </row>
-    <row r="254" spans="1:6">
+      <c r="G253" s="6">
+        <v>14541.9</v>
+      </c>
+      <c r="H253" s="5">
+        <v>9864.7999999999993</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -5719,8 +7245,14 @@
       <c r="F254" s="5">
         <v>526.29999999999995</v>
       </c>
-    </row>
-    <row r="255" spans="1:6">
+      <c r="G254" s="6">
+        <v>14604.8</v>
+      </c>
+      <c r="H254" s="5">
+        <v>9917.7000000000007</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -5739,8 +7271,14 @@
       <c r="F255" s="5">
         <v>522.1</v>
       </c>
-    </row>
-    <row r="256" spans="1:6">
+      <c r="G255" s="6">
+        <v>14745.9</v>
+      </c>
+      <c r="H255" s="5">
+        <v>9998.4</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -5759,8 +7297,14 @@
       <c r="F256" s="5">
         <v>527.79999999999995</v>
       </c>
-    </row>
-    <row r="257" spans="1:6">
+      <c r="G256" s="6">
+        <v>14845.5</v>
+      </c>
+      <c r="H256" s="5">
+        <v>10063.1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -5779,8 +7323,14 @@
       <c r="F257" s="5">
         <v>538.6</v>
       </c>
-    </row>
-    <row r="258" spans="1:6">
+      <c r="G257" s="6">
+        <v>14939</v>
+      </c>
+      <c r="H257" s="5">
+        <v>10166.1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -5799,8 +7349,14 @@
       <c r="F258" s="5">
         <v>535.20000000000005</v>
       </c>
-    </row>
-    <row r="259" spans="1:6">
+      <c r="G258" s="6">
+        <v>14881.3</v>
+      </c>
+      <c r="H258" s="5">
+        <v>10217.1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -5819,8 +7375,14 @@
       <c r="F259" s="5">
         <v>545.70000000000005</v>
       </c>
-    </row>
-    <row r="260" spans="1:6">
+      <c r="G259" s="6">
+        <v>14989.6</v>
+      </c>
+      <c r="H259" s="5">
+        <v>10237.700000000001</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -5839,8 +7401,14 @@
       <c r="F260" s="5">
         <v>552.70000000000005</v>
       </c>
-    </row>
-    <row r="261" spans="1:6">
+      <c r="G260" s="6">
+        <v>15021.1</v>
+      </c>
+      <c r="H260" s="5">
+        <v>10282.200000000001</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -5859,8 +7427,14 @@
       <c r="F261" s="5">
         <v>556.20000000000005</v>
       </c>
-    </row>
-    <row r="262" spans="1:6">
+      <c r="G261" s="6">
+        <v>15190.3</v>
+      </c>
+      <c r="H261" s="5">
+        <v>10316.799999999999</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -5879,8 +7453,14 @@
       <c r="F262" s="5">
         <v>572.4</v>
       </c>
-    </row>
-    <row r="263" spans="1:6">
+      <c r="G262" s="6">
+        <v>15291</v>
+      </c>
+      <c r="H262" s="5">
+        <v>10379</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -5899,8 +7479,14 @@
       <c r="F263" s="5">
         <v>572.5</v>
       </c>
-    </row>
-    <row r="264" spans="1:6">
+      <c r="G263" s="6">
+        <v>15362.4</v>
+      </c>
+      <c r="H263" s="5">
+        <v>10396.6</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -5919,8 +7505,14 @@
       <c r="F264" s="5">
         <v>566.29999999999995</v>
       </c>
-    </row>
-    <row r="265" spans="1:6">
+      <c r="G264" s="6">
+        <v>15380.8</v>
+      </c>
+      <c r="H264" s="5">
+        <v>10424.1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -5939,8 +7531,14 @@
       <c r="F265" s="5">
         <v>580.5</v>
       </c>
-    </row>
-    <row r="266" spans="1:6">
+      <c r="G265" s="6">
+        <v>15384.3</v>
+      </c>
+      <c r="H265" s="5">
+        <v>10453.200000000001</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -5959,8 +7557,14 @@
       <c r="F266" s="5">
         <v>594.1</v>
       </c>
-    </row>
-    <row r="267" spans="1:6">
+      <c r="G266" s="6">
+        <v>15491.9</v>
+      </c>
+      <c r="H266" s="5">
+        <v>10502.3</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -5979,8 +7583,14 @@
       <c r="F267" s="5">
         <v>589.5</v>
       </c>
-    </row>
-    <row r="268" spans="1:6">
+      <c r="G267" s="6">
+        <v>15521.6</v>
+      </c>
+      <c r="H267" s="5">
+        <v>10523.9</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -5999,8 +7609,14 @@
       <c r="F268" s="5">
         <v>593.70000000000005</v>
       </c>
-    </row>
-    <row r="269" spans="1:6">
+      <c r="G268" s="6">
+        <v>15641.3</v>
+      </c>
+      <c r="H268" s="5">
+        <v>10573.1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -6019,8 +7635,14 @@
       <c r="F269" s="5">
         <v>590.1</v>
       </c>
-    </row>
-    <row r="270" spans="1:6">
+      <c r="G269" s="6">
+        <v>15793.9</v>
+      </c>
+      <c r="H269" s="5">
+        <v>10662.2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -6039,8 +7661,14 @@
       <c r="F270" s="5">
         <v>599.79999999999995</v>
       </c>
-    </row>
-    <row r="271" spans="1:6">
+      <c r="G270" s="6">
+        <v>15757.6</v>
+      </c>
+      <c r="H270" s="5">
+        <v>10713.4</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -6059,8 +7687,14 @@
       <c r="F271" s="5">
         <v>618.4</v>
       </c>
-    </row>
-    <row r="272" spans="1:6">
+      <c r="G271" s="6">
+        <v>15935.8</v>
+      </c>
+      <c r="H271" s="5">
+        <v>10805.1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -6079,8 +7713,14 @@
       <c r="F272" s="5">
         <v>621.6</v>
       </c>
-    </row>
-    <row r="273" spans="1:6">
+      <c r="G272" s="6">
+        <v>16139.5</v>
+      </c>
+      <c r="H272" s="5">
+        <v>10909.9</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -6099,8 +7739,14 @@
       <c r="F273" s="5">
         <v>626.9</v>
       </c>
-    </row>
-    <row r="274" spans="1:6">
+      <c r="G273" s="6">
+        <v>16220.2</v>
+      </c>
+      <c r="H273" s="5">
+        <v>11045.2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -6119,8 +7765,14 @@
       <c r="F274" s="5">
         <v>626.79999999999995</v>
       </c>
-    </row>
-    <row r="275" spans="1:6">
+      <c r="G274" s="6">
+        <v>16350</v>
+      </c>
+      <c r="H274" s="5">
+        <v>11145.3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -6139,8 +7791,14 @@
       <c r="F275" s="5">
         <v>629.6</v>
       </c>
-    </row>
-    <row r="276" spans="1:6">
+      <c r="G275" s="6">
+        <v>16460.900000000001</v>
+      </c>
+      <c r="H275" s="5">
+        <v>11227.9</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -6159,8 +7817,14 @@
       <c r="F276" s="5">
         <v>639.9</v>
       </c>
-    </row>
-    <row r="277" spans="1:6">
+      <c r="G276" s="6">
+        <v>16527.599999999999</v>
+      </c>
+      <c r="H276" s="5">
+        <v>11304.6</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -6179,8 +7843,14 @@
       <c r="F277" s="5">
         <v>644.9</v>
       </c>
-    </row>
-    <row r="278" spans="1:6">
+      <c r="G277" s="6">
+        <v>16547.599999999999</v>
+      </c>
+      <c r="H277" s="5">
+        <v>11379.3</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -6199,8 +7869,14 @@
       <c r="F278" s="5">
         <v>643.5</v>
       </c>
-    </row>
-    <row r="279" spans="1:6">
+      <c r="G278" s="6">
+        <v>16571.599999999999</v>
+      </c>
+      <c r="H278" s="5">
+        <v>11430.5</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -6219,8 +7895,14 @@
       <c r="F279" s="5">
         <v>654.20000000000005</v>
       </c>
-    </row>
-    <row r="280" spans="1:6">
+      <c r="G279" s="6">
+        <v>16663.5</v>
+      </c>
+      <c r="H279" s="5">
+        <v>11537.7</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -6239,8 +7921,14 @@
       <c r="F280" s="5">
         <v>662.9</v>
       </c>
-    </row>
-    <row r="281" spans="1:6">
+      <c r="G280" s="6">
+        <v>16778.099999999999</v>
+      </c>
+      <c r="H280" s="5">
+        <v>11618.1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8">
       <c r="A281" t="s">
         <v>280</v>
       </c>
@@ -6259,8 +7947,14 @@
       <c r="F281" s="5">
         <v>666.2</v>
       </c>
-    </row>
-    <row r="282" spans="1:6">
+      <c r="G281" s="6">
+        <v>16851.400000000001</v>
+      </c>
+      <c r="H281" s="5">
+        <v>11702.1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -6279,8 +7973,14 @@
       <c r="F282" s="5">
         <v>674.1</v>
       </c>
-    </row>
-    <row r="283" spans="1:6">
+      <c r="G282" s="6">
+        <v>16903.2</v>
+      </c>
+      <c r="H282" s="5">
+        <v>11758</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -6299,21 +7999,27 @@
       <c r="F283" s="5">
         <v>690.5</v>
       </c>
-    </row>
-    <row r="284" spans="1:6">
+      <c r="G283" s="6">
+        <v>17031.099999999999</v>
+      </c>
+      <c r="H283" s="5">
+        <v>11853</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8">
       <c r="B284" s="2"/>
       <c r="D284" s="4"/>
     </row>
-    <row r="285" spans="1:6">
+    <row r="285" spans="1:8">
       <c r="B285" s="2"/>
     </row>
-    <row r="286" spans="1:6">
+    <row r="286" spans="1:8">
       <c r="B286" s="2"/>
     </row>
-    <row r="287" spans="1:6">
+    <row r="287" spans="1:8">
       <c r="B287" s="2"/>
     </row>
-    <row r="288" spans="1:6">
+    <row r="288" spans="1:8">
       <c r="B288" s="2"/>
     </row>
     <row r="289" spans="2:2">

</xml_diff>